<commit_message>
additional updates for twenty twenty
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6B31D7B-46C1-3C40-AE40-A06772F73F85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA47F42-B25B-744E-863F-FC8EF64F1BAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="1720" windowWidth="29160" windowHeight="18480" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -192,39 +192,12 @@
     <t>Date, Rm</t>
   </si>
   <si>
-    <t>Tues, Aug 27, Rm 270</t>
-  </si>
-  <si>
-    <t>Thurs, Aug 29, Rm CC</t>
-  </si>
-  <si>
-    <t>Tues, Sep 03, Rm 270</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 05, Rm 270</t>
-  </si>
-  <si>
     <t>Tues, Sep 10, Rm 330</t>
   </si>
   <si>
-    <t>Thurs, Sep 12, Rm 270</t>
-  </si>
-  <si>
-    <t>Tues, Sep 17, Rm CC</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 19, Rm CC</t>
-  </si>
-  <si>
     <t>Tues, Sep 24, Rm 330</t>
   </si>
   <si>
-    <t>Thurs, Sep 26, Rm 270</t>
-  </si>
-  <si>
-    <t>Tues, Oct 01, Rm 270</t>
-  </si>
-  <si>
     <t>Thurs, Oct 03, Rm 330</t>
   </si>
   <si>
@@ -234,9 +207,6 @@
     <t>Thurs, Oct 10, Rm 330</t>
   </si>
   <si>
-    <t>Tues, Oct 15, Rm 270</t>
-  </si>
-  <si>
     <t>Thurs, Oct 17, Rm 330</t>
   </si>
   <si>
@@ -246,15 +216,9 @@
     <t>Thurs, Oct 24, Rm 330</t>
   </si>
   <si>
-    <t>Tues, Oct 29, Rm 270</t>
-  </si>
-  <si>
     <t>Thurs, Oct 31, Rm 330</t>
   </si>
   <si>
-    <t>Tues, Nov 05, Rm 270</t>
-  </si>
-  <si>
     <t>Thurs, Nov 07, Rm 330</t>
   </si>
   <si>
@@ -264,13 +228,7 @@
     <t>Thurs, Nov 14, Rm 330</t>
   </si>
   <si>
-    <t>Tues, Nov 19, Rm 270</t>
-  </si>
-  <si>
     <t>Thurs, Nov 21, Rm 330</t>
-  </si>
-  <si>
-    <t>Tues, Nov 26, Rm 270</t>
   </si>
   <si>
     <t xml:space="preserve">Thurs, Nov 28, Rm </t>
@@ -401,6 +359,48 @@
   </si>
   <si>
     <t>- Discuss Final Project</t>
+  </si>
+  <si>
+    <t>Thurs, Aug 29</t>
+  </si>
+  <si>
+    <t>Tues, Sep 17</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 19</t>
+  </si>
+  <si>
+    <t>Tues, Aug 27</t>
+  </si>
+  <si>
+    <t>Tues, Sep 03</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 05</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 12</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 26</t>
+  </si>
+  <si>
+    <t>Tues, Oct 01</t>
+  </si>
+  <si>
+    <t>Tues, Oct 15</t>
+  </si>
+  <si>
+    <t>Tues, Oct 29</t>
+  </si>
+  <si>
+    <t>Tues, Nov 05</t>
+  </si>
+  <si>
+    <t>Tues, Nov 19</t>
+  </si>
+  <si>
+    <t>Tues, Nov 26</t>
   </si>
 </sst>
 </file>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -818,10 +818,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>2</v>
@@ -829,33 +829,33 @@
     </row>
     <row r="3" spans="1:4" ht="127" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>34</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="6" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
@@ -883,7 +883,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>21</v>
@@ -897,7 +897,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>22</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>14</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>28</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>27</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>33</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>6</v>
@@ -1012,23 +1012,23 @@
         <v>18</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>45</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>43</v>
@@ -1037,18 +1037,18 @@
         <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="20" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
         <v>38</v>
@@ -1070,125 +1070,125 @@
     </row>
     <row r="21" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="99" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
didn't get calendar rebuilt and last commit
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA47F42-B25B-744E-863F-FC8EF64F1BAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B90F32A5-FC4C-DE4A-A96C-4B3D57596D7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Topic</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Pandas: Indices &amp; Missing</t>
   </si>
   <si>
-    <t>FALL BREAK</t>
-  </si>
-  <si>
     <t>Collaborating using Github</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
   </si>
   <si>
     <t>Machine Learning with sckikit-learn</t>
-  </si>
-  <si>
-    <t>THANKSGIVING BREAK</t>
   </si>
   <si>
     <t>- JVP pp 149 - 157</t>
@@ -190,48 +184,6 @@
   </si>
   <si>
     <t>Date, Rm</t>
-  </si>
-  <si>
-    <t>Tues, Sep 10, Rm 330</t>
-  </si>
-  <si>
-    <t>Tues, Sep 24, Rm 330</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 03, Rm 330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tues, Oct 08, Rm </t>
-  </si>
-  <si>
-    <t>Thurs, Oct 10, Rm 330</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 17, Rm 330</t>
-  </si>
-  <si>
-    <t>Tues, Oct 22, Rm 330</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 24, Rm 330</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 31, Rm 330</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 07, Rm 330</t>
-  </si>
-  <si>
-    <t>Tues, Nov 12, Rm 330</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 14, Rm 330</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 21, Rm 330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thurs, Nov 28, Rm </t>
   </si>
   <si>
     <t>- Pandas: Reshaping
@@ -293,9 +245,6 @@
   </si>
   <si>
     <t>- Class Introduction</t>
-  </si>
-  <si>
-    <t>Friday Aug 30</t>
   </si>
   <si>
     <t>**SOFTWARE INSTALL DAY**</t>
@@ -361,24 +310,12 @@
     <t>- Discuss Final Project</t>
   </si>
   <si>
-    <t>Thurs, Aug 29</t>
-  </si>
-  <si>
     <t>Tues, Sep 17</t>
   </si>
   <si>
     <t>Thurs, Sep 19</t>
   </si>
   <si>
-    <t>Tues, Aug 27</t>
-  </si>
-  <si>
-    <t>Tues, Sep 03</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 05</t>
-  </si>
-  <si>
     <t>Thurs, Sep 12</t>
   </si>
   <si>
@@ -397,10 +334,61 @@
     <t>Tues, Nov 05</t>
   </si>
   <si>
-    <t>Tues, Nov 19</t>
-  </si>
-  <si>
-    <t>Tues, Nov 26</t>
+    <t>Thurs, Aug 20</t>
+  </si>
+  <si>
+    <t>Tues, Aug 18</t>
+  </si>
+  <si>
+    <t>Fri, Aug 21</t>
+  </si>
+  <si>
+    <t>Tues, Aug 25</t>
+  </si>
+  <si>
+    <t>Thurs, Aug 27</t>
+  </si>
+  <si>
+    <t>Tues, Sep 1</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 3</t>
+  </si>
+  <si>
+    <t>Tues, Sep 10</t>
+  </si>
+  <si>
+    <t>Tues, Sep 24</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 03</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 10</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 17</t>
+  </si>
+  <si>
+    <t>Tues, Oct 22</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 24</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 31</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 07</t>
+  </si>
+  <si>
+    <t>Tues, Nov 12</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 14</t>
+  </si>
+  <si>
+    <t>Tues, Oct 08</t>
   </si>
 </sst>
 </file>
@@ -788,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,7 +792,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -813,15 +801,15 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>2</v>
@@ -829,369 +817,353 @@
     </row>
     <row r="3" spans="1:4" ht="127" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="113" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="C19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="113" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>64</v>
+        <v>99</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="99" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>89</v>
+        <v>101</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>90</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="9"/>
       <c r="D26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>9</v>
+        <v>68</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update welcome video links
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A84942D-A305-0E43-90BD-8C009DC37641}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA374AA-AE0F-2240-86B4-470F32F579A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33720" windowHeight="18500" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -389,8 +389,8 @@
   </si>
   <si>
     <t>- `Student Survey &lt;https://forms.gle/p4z28BLH6TyBRBHg9&gt;`_
-- `Watch Welcome Video &lt;https://www.youtube.com/watch?v=f0awaGKfLEI&gt;`_
-- `What is Data Science &lt;https://www.youtube.com/watch?v=446X6hhXSjo&gt;`_</t>
+- `Watch Welcome Video &lt;https://youtu.be/8IpLNrjINCA&gt;`_
+- `What is Data Science? &lt;https://www.youtube.com/watch?v=446X6hhXSjo&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -806,7 +806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
add office hours and update links
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA374AA-AE0F-2240-86B4-470F32F579A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C05B32-C63A-AE49-9B80-4F803C5C45DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33720" windowHeight="18500" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -250,147 +250,147 @@
     <t>A day of trouble shooting install issues</t>
   </si>
   <si>
-    <t>- `Command Line Basics &lt;command_line_part1.ipynb&gt;`_
-- Read and sign syllabus
+    <t>`Link &lt;exercises/Exercise_git.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_git_2.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>Distributed Computing, Part 3</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>- `Julia for Academic Research &lt;https://www.youtube.com/watch?v=C4dMYHzW-SY&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link 1 &lt;exercises/Exercise_CommandLine_1_Basics.ipynb&gt;`_
+- `Link 2 &lt;exercises/Exercise_CommandLine_2_Advanced.ipynb&gt;`_
+- `Link 3 &lt;exercises/Exercise_jupyterlab.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- Review linear regression as matrix manipulations. `Here's a nice review. &lt;https://www.stat.purdue.edu/~boli/stat512/lectures/topic3.pdf&gt;`_
+- `Review how to define classes &lt;https://realpython.com/python3-object-oriented-programming/&gt;`_</t>
+  </si>
+  <si>
+    <t>- Defining Your Own Estimators</t>
+  </si>
+  <si>
+    <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_
+- `Distributed Computing with dask &lt;distributed_computing.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- Parallelism 
+- Distributed Computing, Part 1</t>
+  </si>
+  <si>
+    <t>**Discuss mid-semester project in class**</t>
+  </si>
+  <si>
+    <t>- JVP pp 331 - 359
+- **Opioid Project Rough Draft Due**</t>
+  </si>
+  <si>
+    <t>**Opioid Project Final Draft Due**</t>
+  </si>
+  <si>
+    <t>- Discuss Final Project</t>
+  </si>
+  <si>
+    <t>Tues, Sep 17</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 19</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 12</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 26</t>
+  </si>
+  <si>
+    <t>Tues, Oct 01</t>
+  </si>
+  <si>
+    <t>Tues, Oct 15</t>
+  </si>
+  <si>
+    <t>Tues, Oct 29</t>
+  </si>
+  <si>
+    <t>Tues, Nov 05</t>
+  </si>
+  <si>
+    <t>Thurs, Aug 20</t>
+  </si>
+  <si>
+    <t>Tues, Aug 18</t>
+  </si>
+  <si>
+    <t>Fri, Aug 21</t>
+  </si>
+  <si>
+    <t>Tues, Aug 25</t>
+  </si>
+  <si>
+    <t>Thurs, Aug 27</t>
+  </si>
+  <si>
+    <t>Tues, Sep 1</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 3</t>
+  </si>
+  <si>
+    <t>Tues, Sep 10</t>
+  </si>
+  <si>
+    <t>Tues, Sep 24</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 03</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 10</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 17</t>
+  </si>
+  <si>
+    <t>Tues, Oct 22</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 24</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 31</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 07</t>
+  </si>
+  <si>
+    <t>Tues, Nov 12</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 14</t>
+  </si>
+  <si>
+    <t>Tues, Oct 08</t>
+  </si>
+  <si>
+    <t>- `Student Survey &lt;https://forms.gle/p4z28BLH6TyBRBHg9&gt;`_
+- `Watch Welcome Video &lt;https://youtu.be/8IpLNrjINCA&gt;`_
+- `What is Data Science? &lt;https://www.youtube.com/watch?v=446X6hhXSjo&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Read and sign syllabus &lt;https://github.com/nickeubank/practicaldatascience/raw/master/syllabus/Syllabus_PracticalDataScience.pdf&gt;`_
 - `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
 - `Register for DataCamp &lt;https://www.datacamp.com/home&gt;`_
+- `Command Line Basics &lt;command_line_part1.ipynb&gt;`_
 - `Advanced Command Line &lt;command_line_part2.ipynb&gt;`_
 - `Setup Python &lt;setup_environment.ipynb&gt;`_
 - `Jupyter Tutorial &lt;jupyter.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>`Link &lt;exercises/Exercise_git.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>`Link &lt;exercises/Exercise_git_2.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>Distributed Computing, Part 3</t>
-  </si>
-  <si>
-    <t>Julia</t>
-  </si>
-  <si>
-    <t>- `Julia for Academic Research &lt;https://www.youtube.com/watch?v=C4dMYHzW-SY&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link 1 &lt;exercises/Exercise_CommandLine_1_Basics.ipynb&gt;`_
-- `Link 2 &lt;exercises/Exercise_CommandLine_2_Advanced.ipynb&gt;`_
-- `Link 3 &lt;exercises/Exercise_jupyterlab.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- Review linear regression as matrix manipulations. `Here's a nice review. &lt;https://www.stat.purdue.edu/~boli/stat512/lectures/topic3.pdf&gt;`_
-- `Review how to define classes &lt;https://realpython.com/python3-object-oriented-programming/&gt;`_</t>
-  </si>
-  <si>
-    <t>- Defining Your Own Estimators</t>
-  </si>
-  <si>
-    <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_
-- `Distributed Computing with dask &lt;distributed_computing.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- Parallelism 
-- Distributed Computing, Part 1</t>
-  </si>
-  <si>
-    <t>**Discuss mid-semester project in class**</t>
-  </si>
-  <si>
-    <t>- JVP pp 331 - 359
-- **Opioid Project Rough Draft Due**</t>
-  </si>
-  <si>
-    <t>**Opioid Project Final Draft Due**</t>
-  </si>
-  <si>
-    <t>- Discuss Final Project</t>
-  </si>
-  <si>
-    <t>Tues, Sep 17</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 19</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 12</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 26</t>
-  </si>
-  <si>
-    <t>Tues, Oct 01</t>
-  </si>
-  <si>
-    <t>Tues, Oct 15</t>
-  </si>
-  <si>
-    <t>Tues, Oct 29</t>
-  </si>
-  <si>
-    <t>Tues, Nov 05</t>
-  </si>
-  <si>
-    <t>Thurs, Aug 20</t>
-  </si>
-  <si>
-    <t>Tues, Aug 18</t>
-  </si>
-  <si>
-    <t>Fri, Aug 21</t>
-  </si>
-  <si>
-    <t>Tues, Aug 25</t>
-  </si>
-  <si>
-    <t>Thurs, Aug 27</t>
-  </si>
-  <si>
-    <t>Tues, Sep 1</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 3</t>
-  </si>
-  <si>
-    <t>Tues, Sep 10</t>
-  </si>
-  <si>
-    <t>Tues, Sep 24</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 03</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 10</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 17</t>
-  </si>
-  <si>
-    <t>Tues, Oct 22</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 24</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 31</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 07</t>
-  </si>
-  <si>
-    <t>Tues, Nov 12</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 14</t>
-  </si>
-  <si>
-    <t>Tues, Oct 08</t>
-  </si>
-  <si>
-    <t>- `Student Survey &lt;https://forms.gle/p4z28BLH6TyBRBHg9&gt;`_
-- `Watch Welcome Video &lt;https://youtu.be/8IpLNrjINCA&gt;`_
-- `What is Data Science? &lt;https://www.youtube.com/watch?v=446X6hhXSjo&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -781,14 +781,14 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="48" style="8" customWidth="1"/>
+    <col min="3" max="3" width="67.1640625" style="8" customWidth="1"/>
     <col min="4" max="4" width="57.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -808,32 +808,32 @@
     </row>
     <row r="2" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="127" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>61</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>31</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="6" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>2</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>18</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>19</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>3</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>25</v>
@@ -957,7 +957,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>24</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>30</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
@@ -994,23 +994,23 @@
         <v>15</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>40</v>
@@ -1019,12 +1019,12 @@
         <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="19" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>44</v>
@@ -1052,7 +1052,7 @@
     </row>
     <row r="20" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>46</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="21" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
@@ -1080,13 +1080,13 @@
     </row>
     <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
         <v>52</v>
@@ -1094,13 +1094,13 @@
     </row>
     <row r="23" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
         <v>53</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>56</v>
@@ -1119,13 +1119,13 @@
     </row>
     <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
         <v>57</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" t="s">
         <v>55</v>
@@ -1145,27 +1145,27 @@
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="D28" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move advanced command line back
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C05B32-C63A-AE49-9B80-4F803C5C45DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51CBF93-6A5F-3448-B7DD-ADD723DDDC47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33720" windowHeight="18500" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Topic</t>
   </si>
@@ -256,18 +258,10 @@
     <t>`Link &lt;exercises/Exercise_git_2.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>Distributed Computing, Part 3</t>
-  </si>
-  <si>
     <t>Julia</t>
   </si>
   <si>
     <t>- `Julia for Academic Research &lt;https://www.youtube.com/watch?v=C4dMYHzW-SY&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link 1 &lt;exercises/Exercise_CommandLine_1_Basics.ipynb&gt;`_
-- `Link 2 &lt;exercises/Exercise_CommandLine_2_Advanced.ipynb&gt;`_
-- `Link 3 &lt;exercises/Exercise_jupyterlab.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- Review linear regression as matrix manipulations. `Here's a nice review. &lt;https://www.stat.purdue.edu/~boli/stat512/lectures/topic3.pdf&gt;`_
@@ -290,9 +284,6 @@
   <si>
     <t>- JVP pp 331 - 359
 - **Opioid Project Rough Draft Due**</t>
-  </si>
-  <si>
-    <t>**Opioid Project Final Draft Due**</t>
   </si>
   <si>
     <t>- Discuss Final Project</t>
@@ -382,15 +373,30 @@
     <t>- `Student Survey &lt;https://forms.gle/p4z28BLH6TyBRBHg9&gt;`_
 - `Watch Welcome Video &lt;https://youtu.be/8IpLNrjINCA&gt;`_
 - `What is Data Science? &lt;https://www.youtube.com/watch?v=446X6hhXSjo&gt;`_</t>
+  </si>
+  <si>
+    <t>- Advanced Command Line</t>
   </si>
   <si>
     <t>- `Read and sign syllabus &lt;https://github.com/nickeubank/practicaldatascience/raw/master/syllabus/Syllabus_PracticalDataScience.pdf&gt;`_
 - `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
 - `Register for DataCamp &lt;https://www.datacamp.com/home&gt;`_
 - `Command Line Basics &lt;command_line_part1.ipynb&gt;`_
-- `Advanced Command Line &lt;command_line_part2.ipynb&gt;`_
 - `Setup Python &lt;setup_environment.ipynb&gt;`_
 - `Jupyter Tutorial &lt;jupyter.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Advanced Command Line &lt;command_line_part2.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link 1 &lt;exercises/Exercise_CommandLine_1_Basics.ipynb&gt;`_
+- `Link 2 &lt;exercises/Exercise_jupyterlab.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;exercises/Exercise_CommandLine_2_Advanced.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>**OPIOID PROJECT DUE**</t>
   </si>
 </sst>
 </file>
@@ -780,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -808,32 +814,32 @@
     </row>
     <row r="2" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="127" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>61</v>
@@ -843,329 +849,334 @@
       </c>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="71" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="3" t="s">
+    <row r="7" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="113" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="113" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="119" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="9" t="s">
+      <c r="B26" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C28" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="D28" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add parquet, update storage with azcopy, more building
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E35A710-7AAD-904F-B884-614A2ADC6ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC747F5-E2B7-3742-A0DC-8706A6C1D801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11500" yWindow="460" windowWidth="23340" windowHeight="18500" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -125,11 +125,6 @@
 - Getting Help Online</t>
   </si>
   <si>
-    <t>- `What is Big Data? &lt;what_is_big_data.ipynb&gt;`_
-- `Strategies for Big Data &lt;big_data_strategies.ipynb&gt;`_
-- Download the dataset linked at the top of the linked exercise before class.</t>
-  </si>
-  <si>
     <t>Git and Github 2</t>
   </si>
   <si>
@@ -138,12 +133,6 @@
   <si>
     <t>- Pandas: Reshaping
 - Pandas: Categoricals</t>
-  </si>
-  <si>
-    <t>- WM 8.3
-- `Pandas reshaping (with pics!) &lt;https://pandas.pydata.org/pandas-docs/stable/user_guide/reshaping.html&gt;`_
-- `What is goal of reshaping? &lt;https://www.jstatsoft.org/index.php/jss/article/view/v059i10/v59i10.pdf&gt;`_
-- Categoricals: WM 12.1</t>
   </si>
   <si>
     <t>Speed and Performance in Python</t>
@@ -401,6 +390,19 @@
 - IF did not complete DataCamp: Do Numpy Section
 - `Numbers in Computer &lt;ints_and_floats.ipynb&gt;`_
 - `OPTIONAL: How numpy works &lt;https://www.nature.com/articles/s41586-020-2649-2&gt;`_</t>
+  </si>
+  <si>
+    <t>- `What is Big Data? &lt;what_is_big_data.ipynb&gt;`_
+- `Strategies for Big Data &lt;big_data_strategies.ipynb&gt;`_
+- Download the dataset linked at the top of the linked exercise before class.
+- `Parquet Format &lt;parquet.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- WM 8.3
+- `Pandas reshaping (with pics!) &lt;https://pandas.pydata.org/pandas-docs/stable/user_guide/reshaping.html&gt;`_
+- `What is goal of reshaping? &lt;https://www.jstatsoft.org/index.php/jss/article/view/v059i10/v59i10.pdf&gt;`_
+- Categoricals: WM 12.1
+- **Project Strategy Plan Due**</t>
   </si>
 </sst>
 </file>
@@ -790,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,7 +806,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -818,64 +820,64 @@
     </row>
     <row r="2" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
@@ -883,13 +885,13 @@
     </row>
     <row r="7" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>9</v>
@@ -897,7 +899,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
@@ -911,7 +913,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -925,21 +927,21 @@
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>3</v>
@@ -953,13 +955,13 @@
     </row>
     <row r="12" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>10</v>
@@ -967,27 +969,27 @@
     </row>
     <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>26</v>
@@ -995,7 +997,7 @@
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
@@ -1004,177 +1006,177 @@
         <v>8</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="99" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add arcos on azure exercise
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEC0E73-06E6-BF49-B0D7-7087CBA24143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024B64F4-1336-3846-A75A-0816FD662642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="460" windowWidth="29200" windowHeight="19760" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="11260" yWindow="460" windowWidth="29200" windowHeight="19740" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Topic</t>
   </si>
@@ -195,10 +195,6 @@
   <si>
     <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_
 - `Distributed Computing with dask &lt;distributed_computing.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- Parallelism 
-- Distributed Computing, Part 1</t>
   </si>
   <si>
     <t>**Discuss mid-semester project in class**</t>
@@ -396,13 +392,6 @@
     <t>Distributed Computing, Azure 2</t>
   </si>
   <si>
-    <t>**OPIOID PROJECT DUE (Extensions available upon request to assigned date for PDS final)**</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_dask.ipynb&gt;`_
-- `Link &lt;exercises/Exercise_dask_realdata.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
@@ -410,6 +399,22 @@
   </si>
   <si>
     <t>`Julia &lt;https://www.youtube.com/watch?v=C4dMYHzW-SY&gt;`_</t>
+  </si>
+  <si>
+    <t>- Parallelism 
+- Distributed Computing</t>
+  </si>
+  <si>
+    <t>- `Link 1 &lt;exercises/Exercise_dask.ipynb&gt;`_
+- `Link 2 &lt;exercises/Exercise_dask_realdata.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_azure_arcos.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- **OPIOID PROJECT DUE (Extensions available upon request to assigned date for PDS final)**
+- `Azure Storage &lt;cloud_azurestorage.ipynb&gt;`_
+- `More Azure Concepts &lt;cloud_more_concepts.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -800,7 +805,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -827,32 +832,32 @@
     </row>
     <row r="2" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>42</v>
@@ -864,27 +869,27 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
@@ -892,13 +897,13 @@
     </row>
     <row r="7" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>9</v>
@@ -906,7 +911,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
@@ -920,7 +925,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -934,21 +939,21 @@
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>3</v>
@@ -962,13 +967,13 @@
     </row>
     <row r="12" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>10</v>
@@ -976,13 +981,13 @@
     </row>
     <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>21</v>
@@ -990,13 +995,13 @@
     </row>
     <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>26</v>
@@ -1004,7 +1009,7 @@
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
@@ -1018,7 +1023,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>28</v>
@@ -1029,21 +1034,21 @@
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
@@ -1057,13 +1062,13 @@
     </row>
     <row r="19" spans="1:4" ht="141" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>23</v>
@@ -1071,7 +1076,7 @@
     </row>
     <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>31</v>
@@ -1085,7 +1090,7 @@
     </row>
     <row r="21" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
@@ -1099,13 +1104,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" t="s">
         <v>37</v>
@@ -1113,7 +1118,7 @@
     </row>
     <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>47</v>
@@ -1127,68 +1132,71 @@
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>102</v>
+      <c r="C28" s="9" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D29" s="10"/>
     </row>

</xml_diff>

<commit_message>
update azure to cli
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F051F0DD-0996-174C-90A6-C0C6CA0780A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB11BD39-93DB-B14E-A600-DF0CA35E1670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9200" yWindow="460" windowWidth="29200" windowHeight="19740" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -396,11 +396,6 @@
     <t>`Link &lt;exercises/Exercise_azure_arcos.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- **OPIOID PROJECT DUE (Extensions available upon request to assigned date for PDS final)**
-- `Azure Storage &lt;cloud_azurestorage.ipynb&gt;`_
-- `More Azure Concepts &lt;cloud_more_concepts.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>`Link 1 &lt;exercises/Exercise_dask.ipynb&gt;`_
 `Link 2 &lt;exercises/Exercise_dask_realdata.ipynb&gt;`_</t>
   </si>
@@ -415,6 +410,11 @@
     <t>- `What is The Cloud &lt;cloud_what_is_it.ipynb&gt;`_
 - `Getting Setup on Azure &lt;cloud_azureml.ipynb&gt;`_
 - `Dask on Azure &lt;cloud_dask.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- **OPIOID PROJECT DUE (Extensions available upon request to assigned date for PDS final)**
+- `Azure from Command Line &lt;cloud_azure_cli.ipynb&gt;`_
+- `More Azure Concepts &lt;cloud_more_concepts.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -804,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -852,7 +852,7 @@
         <v>59</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -878,7 +878,7 @@
         <v>60</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -1160,7 +1160,7 @@
         <v>48</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1171,7 +1171,7 @@
         <v>96</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
         <v>102</v>
@@ -1185,7 +1185,7 @@
         <v>97</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
setting up for 2021
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D6E7F323-DD30-4846-B21B-AE6EB484E109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C5C650-A27F-A542-A3D1-24586CB18ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14620" yWindow="760" windowWidth="29200" windowHeight="19740" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="11760" yWindow="500" windowWidth="29200" windowHeight="19740" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
 - `Views and Copies in Pandas &lt;views_and_copies_in_pandas.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>`Link &lt;exercises/Exercise_variables_v_objects.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>`Link &lt;exercises/Exercise_dataframe.ipynb&gt;`_</t>
   </si>
   <si>
@@ -208,14 +205,6 @@
     <t>- Advanced Command Line</t>
   </si>
   <si>
-    <t>- `Read and sign syllabus &lt;https://github.com/nickeubank/practicaldatascience/raw/master/syllabus/Syllabus_PracticalDataScience.pdf&gt;`_
-- `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
-- `Register for DataCamp &lt;https://www.datacamp.com/home&gt;`_
-- `Command Line Basics &lt;command_line_part1.ipynb&gt;`_
-- `Setup Python &lt;setup_environment.ipynb&gt;`_
-- `Jupyter Tutorial &lt;jupyter.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `Advanced Command Line &lt;command_line_part2.ipynb&gt;`_</t>
   </si>
   <si>
@@ -226,12 +215,6 @@
     <t>- IPython
 - Packages
 - Python v. R / variables as pointers</t>
-  </si>
-  <si>
-    <t>- `Follow this link &lt;https://gke.mybinder.org/v2/gh/ipython/ipython-in-depth/master?filepath=binder/Index.ipynb&gt;`_ , then click "Ipython - Beyond plain python" and read that notebook. 
-- `Python packages &lt;managing_python_packages.ipynb&gt;`_
-- `variables v objects &lt;vars_v_objects.ipynb&gt;`_
-- `Python v. R &lt;https://www.practicaldatascience.org/html/python_v_r.html&gt;`_</t>
   </si>
   <si>
     <t>- Understanding Tracebacks
@@ -290,10 +273,6 @@
 `Link 2 &lt;exercises/Exercise_dask_realdata.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>`Link 1 &lt;exercises/Exercise_CommandLine_1_Basics.ipynb&gt;`_
-`Link 2 &lt;exercises/Exercise_jupyterlab.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>`Link &lt;exercises/Exercise_CommandLine_2_Advanced.ipynb&gt;`_</t>
   </si>
   <si>
@@ -388,19 +367,6 @@
   </si>
   <si>
     <t>Spatial Data (GIS)</t>
-  </si>
-  <si>
-    <t>- Spatial Data Types
-- Coordinate Reference Systems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- **OPIOID PROJECT DUE (Extensions available upon request to assigned date for PDS final)**
-- Relating Data Spatially
-- Mapping Spatial Data
-</t>
-  </si>
-  <si>
-    <t>- Advanced GIS Uses</t>
   </si>
   <si>
     <t>- LAST CLASS 
@@ -418,6 +384,45 @@
   </si>
   <si>
     <t>IN PROGRESS</t>
+  </si>
+  <si>
+    <t>- Relating Data Spatially
+- Advanced GIS Uses</t>
+  </si>
+  <si>
+    <t>- `What is GIS? &lt;what_is_gis.ipynb&gt;`_
+- `Installing Geopandas &lt;setup_geopandas.ipynb&gt;`_
+- Vector Data
+- `Raster Data &lt;https://carpentries-incubator.github.io/geospatial-python/01-intro-raster-data/index.html&gt;`_
+- `GeoPandas User Guide: Data Structures, Reading and Writing Files, and Indexing and Selecting Data &lt;https://geopandas.org/docs/user_guide.html&gt;`_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- **OPIOID PROJECT DUE (Extensions available upon request to assigned date for PDS final)**
+- What are Coordinate Reference Systems?
+- `Managing Projections in Geopandas &lt;https://geopandas.org/docs/user_guide/projections.html&gt;`_
+- `Mapping Spatial Data in Geopandas &lt;https://geopandas.org/docs/user_guide/mapping.html&gt;`_
+</t>
+  </si>
+  <si>
+    <t>- `Read and sign syllabus &lt;https://github.com/nickeubank/practicaldatascience/raw/master/syllabus/Syllabus_PracticalDataScience.pdf&gt;`_
+- `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
+- `Register for DataCamp &lt;https://www.datacamp.com/home&gt;`_
+- `Setting Up Your Computer for Data Science &lt;setting_up_your_computer.ipynb&gt;`_
+- `Command Line Basics &lt;command_line_part1.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Follow this link &lt;https://gke.mybinder.org/v2/gh/ipython/ipython-in-depth/master?filepath=binder/Index.ipynb&gt;`_ , then click "Ipython - Beyond plain python" and read that notebook. 
+- `Jupyter Tutorial &lt;jupyter.ipynb&gt;`_
+- `Python packages &lt;managing_python_packages.ipynb&gt;`_
+- `variables v objects &lt;vars_v_objects.ipynb&gt;`_
+- `Python v. R &lt;https://www.practicaldatascience.org/html/python_v_r.html&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link 1 &lt;exercises/Exercise_CommandLine_1_Basics.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link 1 &lt;exercises/Exercise_jupyterlab.ipynb&gt;`_
+`Link 2 &lt;exercises/Exercise_variables_v_objects.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -824,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -838,7 +843,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -852,79 +857,79 @@
     </row>
     <row r="2" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="9"/>
     </row>
-    <row r="3" spans="1:4" ht="99" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="71" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>18</v>
+        <v>106</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>9</v>
@@ -932,7 +937,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
@@ -946,7 +951,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -955,26 +960,26 @@
         <v>14</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>3</v>
@@ -983,18 +988,18 @@
         <v>17</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>10</v>
@@ -1002,43 +1007,43 @@
     </row>
     <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
@@ -1047,189 +1052,189 @@
         <v>8</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="99" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="D21" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="10" t="s">
+      <c r="B29" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="D28" s="9"/>
-    </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" t="s">
         <v>99</v>
       </c>
-      <c r="B30" t="s">
-        <v>106</v>
-      </c>
       <c r="C30" s="9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move to material theme
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB1482B-73B3-5144-88D6-E6E9F6E5F0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A609A592-AFE0-A545-BF4A-42C8D47CF6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5660" yWindow="500" windowWidth="29200" windowHeight="19740" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -365,20 +365,6 @@
 - Advanced GIS Uses</t>
   </si>
   <si>
-    <t>- `What is GIS? &lt;what_is_gis.ipynb&gt;`_
-- `Installing Geopandas &lt;setup_geopandas.ipynb&gt;`_
-- Vector Data
-- `Raster Data &lt;https://carpentries-incubator.github.io/geospatial-python/01-intro-raster-data/index.html&gt;`_
-- `GeoPandas User Guide: Data Structures, Reading and Writing Files, and Indexing and Selecting Data &lt;https://geopandas.org/docs/user_guide.html&gt;`_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- **OPIOID PROJECT DUE (Extensions available upon request to assigned date for PDS final)**
-- What are Coordinate Reference Systems?
-- `Managing Projections in Geopandas &lt;https://geopandas.org/docs/user_guide/projections.html&gt;`_
-- `Mapping Spatial Data in Geopandas &lt;https://geopandas.org/docs/user_guide/mapping.html&gt;`_
-</t>
-  </si>
-  <si>
     <t>- `Follow this link &lt;https://gke.mybinder.org/v2/gh/ipython/ipython-in-depth/master?filepath=binder/Index.ipynb&gt;`_ , then click "Ipython - Beyond plain python" and read that notebook. 
 - `Jupyter Tutorial &lt;jupyter.ipynb&gt;`_
 - `Python packages &lt;managing_python_packages.ipynb&gt;`_
@@ -426,6 +412,21 @@
   <si>
     <t>- Grammer of Graphics
 - Intro to Plotting with Altair</t>
+  </si>
+  <si>
+    <t>- `What is GIS? &lt;gis_what_is_gis.ipynb&gt;`_
+- `Installing Geopandas &lt;gis_setup_geopandas.ipynb&gt;`_
+- Vector Data
+- `Raster Data &lt;https://carpentries-incubator.github.io/geospatial-python/01-intro-raster-data/index.html&gt;`_
+- `GeoPandas User Guide: Data Structures, Reading and Writing Files, and Indexing and Selecting Data &lt;https://geopandas.org/docs/user_guide.html&gt;`_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- **OPIOID PROJECT DUE (Extensions available upon request to assigned date for PDS final)**
+- `Projections and Coordinate Reference Systems &lt;gis_coordinate_reference_systems.ipynb&gt;`_
+- `Managing Projections in Geopandas &lt;https://geopandas.org/docs/user_guide/projections.html&gt;`_
+- `Mapping with Geopandas &lt;gis_plotting.ipynb&gt;`_
+- `Mapping Spatial Data in Geopandas &lt;https://geopandas.org/docs/user_guide/mapping.html&gt;`_
+</t>
   </si>
 </sst>
 </file>
@@ -836,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,10 +871,10 @@
         <v>40</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -884,10 +885,10 @@
         <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -910,10 +911,10 @@
         <v>49</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57" x14ac:dyDescent="0.2">
@@ -963,13 +964,13 @@
         <v>68</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -977,13 +978,13 @@
         <v>69</v>
       </c>
       <c r="B10" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>106</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43" x14ac:dyDescent="0.2">
@@ -1208,10 +1209,10 @@
         <v>91</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>87</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>91</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="D28" s="9"/>
     </row>

</xml_diff>

<commit_message>
update schedule, add homework guidelines
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE92194-DB6F-5440-8370-F55404A35DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86A1DF0-E1C7-1747-82F7-57B4B046A8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30440" windowHeight="17360" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32340" windowHeight="19800" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -53,10 +53,6 @@
     <t>- `Pandas 2: DataFrames &lt;pandas_dataframes.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- Pandas: Loading and saving data
-- Pandas: Cleaning</t>
-  </si>
-  <si>
     <t>- Defensive Programming
 - Workflow
 - Getting Help Online</t>
@@ -116,25 +112,10 @@
     <t>**Discuss mid-semester project in class**</t>
   </si>
   <si>
-    <t>- Understanding Tracebacks
-- Pandas: Merging</t>
-  </si>
-  <si>
-    <t>- JVP pp 149 - 157
-- `What are Tracebacks? &lt;https://www.youtube.com/watch?v=JD8BrXXNtjA&gt;`_</t>
-  </si>
-  <si>
     <t>- `Defensive Programming &lt;defensive_programming.ipynb&gt;`_
 - `Iceberg Principle &lt;iceberg_principle.ipynb&gt;`_
 - `Workflow Management &lt;workflow.ipynb&gt;`_
 - `Getting Help &lt;getting_help.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- WM Chapter 6
-- WM Chapter 7
-- `Python Strings (string section only!) &lt;https://realpython.com/python-data-types/#strings&gt;`_
-- `Identifying Problems &lt;cleaning_identifying.ipynb&gt;`_
-- `Editing Values &lt;cleaning_editingvalues.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- `What is Big Data? &lt;what_is_big_data.ipynb&gt;`_
@@ -433,7 +414,26 @@
     <t>- WM pp 136-142
 - JVP pp 115-139
 - `Views and Copies in Pandas &lt;views_and_copies_in_pandas.ipynb&gt;`_
-- `VS Code Livesharing &lt;https://www.youtube.com/watch?v=2CTi9THB0b4&gt;`_</t>
+- `VS Code Livesharing (first half) &lt;https://www.youtube.com/watch?v=2CTi9THB0b4&gt;`_</t>
+  </si>
+  <si>
+    <t>- JVP pp 149 - 157</t>
+  </si>
+  <si>
+    <t>- WM Chapter 6
+- WM Chapter 7
+- `Python Strings (string section only!) &lt;https://realpython.com/python-data-types/#strings&gt;`_
+- `Identifying Problems &lt;cleaning_identifying.ipynb&gt;`_
+- `Editing Values &lt;cleaning_editingvalues.ipynb&gt;`_
+- `What are Tracebacks? &lt;https://www.youtube.com/watch?v=JD8BrXXNtjA&gt;`_</t>
+  </si>
+  <si>
+    <t>- Pandas: Loading and saving data
+- Pandas: Cleaning
+- Tracebacks</t>
+  </si>
+  <si>
+    <t>- Pandas: Merging</t>
   </si>
 </sst>
 </file>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,7 +857,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -871,389 +871,389 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="C13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="71" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="99" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of updates to plotting
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CA3A80-90FC-9B49-AFBB-CB4F0FD1B6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7589C3-E079-DC4F-8B7B-851EBC549920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32340" windowHeight="19680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -258,10 +258,6 @@
     <t>- Advanced Plotting</t>
   </si>
   <si>
-    <t>- `Principles of Data Visualization &lt;https://www.youtube.com/watch?v=vTingdk_pVM&gt;`_
-- `Intro to Altair &lt;plotting_altair_part1.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- Advanced Altair &lt;plotting_altair_part2.ipynb&gt;`_</t>
   </si>
   <si>
@@ -435,6 +431,11 @@
   <si>
     <t>- `Git and Github &lt;git_and_github.ipynb&gt;`_
 - `Homework Guidelines &lt;homework_guidelines.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Principles of Data Visualization &lt;https://www.youtube.com/watch?v=vTingdk_pVM&gt;`_
+- `Intro to Altair &lt;plotting_altair_part1.ipynb&gt;`_
+- `Altair in Context &lt;plotting_altair_in_context.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -845,7 +846,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,10 +879,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -915,13 +916,13 @@
         <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="71" x14ac:dyDescent="0.2">
@@ -929,13 +930,13 @@
         <v>31</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -943,13 +944,13 @@
         <v>32</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -957,13 +958,13 @@
         <v>33</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.2">
@@ -971,13 +972,13 @@
         <v>34</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.2">
@@ -985,13 +986,13 @@
         <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -999,11 +1000,11 @@
         <v>36</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="71" x14ac:dyDescent="0.2">
@@ -1011,27 +1012,27 @@
         <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1042,10 +1043,10 @@
         <v>63</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1061,13 +1062,13 @@
         <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.2">
@@ -1075,13 +1076,13 @@
         <v>42</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.2">
@@ -1103,13 +1104,13 @@
         <v>44</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="99" x14ac:dyDescent="0.2">
@@ -1123,7 +1124,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.2">
@@ -1131,7 +1132,7 @@
         <v>46</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>8</v>
@@ -1145,13 +1146,13 @@
         <v>47</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1159,13 +1160,13 @@
         <v>48</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
@@ -1179,7 +1180,7 @@
         <v>17</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
@@ -1205,7 +1206,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.2">
@@ -1213,13 +1214,13 @@
         <v>52</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.2">
@@ -1227,10 +1228,10 @@
         <v>53</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" s="8"/>
     </row>

</xml_diff>

<commit_message>
add plotting exercise 3
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85E66BA-E746-2640-AA2B-61A56365EB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656CF42F-ADBA-3E48-83F5-1CB3B832D85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="500" windowWidth="32340" windowHeight="19680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="3680" yWindow="940" windowWidth="32340" windowHeight="19680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule_xlsx" sheetId="1" r:id="rId1"/>
@@ -331,9 +331,6 @@
     <t>- `Link &lt;exercises/Exercise_plotting_part1.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `Link &lt;exercises/Exercise_plotting_part2.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `Link 1 &lt;exercises/Exercise_indices.ipynb&gt;`_
 - `Link 2 &lt;exercises/Exercise_missing.ipynb&gt;`_</t>
   </si>
@@ -436,6 +433,10 @@
   </si>
   <si>
     <t>- `Advanced Altair &lt;plotting_altair_part2.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;exercises/Exercise_plotting_part2.ipynb&gt;`_
+- `Link &lt;exercises/Exercise_plotting_part3.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -846,7 +847,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,13 +917,13 @@
         <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="71" x14ac:dyDescent="0.2">
@@ -933,7 +934,7 @@
         <v>69</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>81</v>
@@ -975,10 +976,10 @@
         <v>72</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.2">
@@ -989,10 +990,10 @@
         <v>74</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1004,7 +1005,7 @@
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="71" x14ac:dyDescent="0.2">
@@ -1012,13 +1013,13 @@
         <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
@@ -1029,13 +1030,13 @@
         <v>64</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>39</v>
       </c>
@@ -1043,10 +1044,10 @@
         <v>63</v>
       </c>
       <c r="C14" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>110</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1062,13 +1063,13 @@
         <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.2">
@@ -1082,7 +1083,7 @@
         <v>22</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.2">
@@ -1110,7 +1111,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="99" x14ac:dyDescent="0.2">
@@ -1124,7 +1125,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.2">
@@ -1152,7 +1153,7 @@
         <v>10</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1166,7 +1167,7 @@
         <v>24</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
@@ -1180,7 +1181,7 @@
         <v>17</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
@@ -1206,7 +1207,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.2">
@@ -1220,7 +1221,7 @@
         <v>65</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
tweak code your own
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33E2C31-B455-F847-AB1C-FAF41FFE0712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{18242A8E-6D59-8842-BEFC-DEF647B3059A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="500" windowWidth="32340" windowHeight="19560" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="3660" yWindow="500" windowWidth="32340" windowHeight="19560" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
-    <sheet name="class_schedule_xlsx" sheetId="1" r:id="rId1"/>
+    <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -221,13 +221,6 @@
 - Intro to Plotting with Altair</t>
   </si>
   <si>
-    <t>- `What is GIS? &lt;gis_what_is_gis.ipynb&gt;`_
-- `Installing Geopandas &lt;gis_setup_geopandas.ipynb&gt;`_
-- Vector Data
-- `Raster Data &lt;https://carpentries-incubator.github.io/geospatial-python/01-intro-raster-data/index.html&gt;`_
-- `GeoPandas User Guide: Data Structures, Reading and Writing Files, and Indexing and Selecting Data &lt;https://geopandas.org/docs/user_guide.html&gt;`_</t>
-  </si>
-  <si>
     <t xml:space="preserve">- **OPIOID PROJECT DUE (Extensions available upon request to assigned date for PDS final)**
 - `Projections and Coordinate Reference Systems &lt;projections_and_crs.ipynb&gt;`_
 - `Managing Projections in Geopandas &lt;https://geopandas.org/docs/user_guide/projections.html&gt;`_
@@ -437,6 +430,12 @@
     <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_
 - `Distributed Computing with dask &lt;distributed_computing.ipynb&gt;`_
 (Note reading includes a 45 minute video to watch)</t>
+  </si>
+  <si>
+    <t>- `What is GIS? &lt;gis_what_is_gis.ipynb&gt;`_
+- `Installing Geopandas &lt;gis_setup_geopandas.ipynb&gt;`_
+- `Geopandas / Vector Data &lt;gis_geopandas.ipynb&gt;`_
+- `GeoPandas User Guide: Data Structures, Reading and Writing Files, and Indexing and Selecting Data &lt;https://geopandas.org/docs/user_guide.html&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -846,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,10 +879,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -917,13 +916,13 @@
         <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="71" x14ac:dyDescent="0.2">
@@ -931,13 +930,13 @@
         <v>22</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -945,13 +944,13 @@
         <v>23</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -959,13 +958,13 @@
         <v>24</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.2">
@@ -973,13 +972,13 @@
         <v>25</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.2">
@@ -987,13 +986,13 @@
         <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1001,11 +1000,11 @@
         <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="71" x14ac:dyDescent="0.2">
@@ -1013,13 +1012,13 @@
         <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
@@ -1030,10 +1029,10 @@
         <v>55</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1044,10 +1043,10 @@
         <v>54</v>
       </c>
       <c r="C14" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>100</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1071,13 +1070,13 @@
         <v>33</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.2">
@@ -1085,13 +1084,13 @@
         <v>34</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.2">
@@ -1099,10 +1098,10 @@
         <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>103</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>13</v>
@@ -1113,13 +1112,13 @@
         <v>36</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="99" x14ac:dyDescent="0.2">
@@ -1133,7 +1132,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.2">
@@ -1141,10 +1140,10 @@
         <v>38</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>8</v>
@@ -1155,13 +1154,13 @@
         <v>39</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1169,13 +1168,13 @@
         <v>40</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
@@ -1183,13 +1182,13 @@
         <v>41</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="D25" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
@@ -1200,24 +1199,24 @@
         <v>17</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.2">
@@ -1225,10 +1224,10 @@
         <v>44</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="8"/>
     </row>

</xml_diff>

<commit_message>
update schedule and solutions
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18242A8E-6D59-8842-BEFC-DEF647B3059A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C56379-09C4-6C40-9B80-9C3EA6E00F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="500" windowWidth="32340" windowHeight="19560" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="3660" yWindow="500" windowWidth="32340" windowHeight="19520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
   <si>
     <t>Topic</t>
   </si>
@@ -189,18 +189,10 @@
     <t>Wed, Dec 8</t>
   </si>
   <si>
-    <t>- LAST CLASS 
-- Spatial Data (GIS)</t>
-  </si>
-  <si>
     <t>Last date things can be submitted</t>
   </si>
   <si>
     <t>(no class)</t>
-  </si>
-  <si>
-    <t>- Relating Data Spatially
-- Advanced GIS Uses</t>
   </si>
   <si>
     <t>- `Read and sign syllabus &lt;https://github.com/nickeubank/practicaldatascience/raw/master/syllabus/Syllabus_PracticalDataScience.pdf&gt;`_
@@ -436,6 +428,13 @@
 - `Installing Geopandas &lt;gis_setup_geopandas.ipynb&gt;`_
 - `Geopandas / Vector Data &lt;gis_geopandas.ipynb&gt;`_
 - `GeoPandas User Guide: Data Structures, Reading and Writing Files, and Indexing and Selecting Data &lt;https://geopandas.org/docs/user_guide.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- Spatial Data (GIS)
+- LAST CLASS</t>
+  </si>
+  <si>
+    <t>More time on defining classes</t>
   </si>
 </sst>
 </file>
@@ -845,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -879,10 +878,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -893,10 +892,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -916,13 +915,13 @@
         <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="D5" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="71" x14ac:dyDescent="0.2">
@@ -930,13 +929,13 @@
         <v>22</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -944,13 +943,13 @@
         <v>23</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -958,13 +957,13 @@
         <v>24</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.2">
@@ -972,13 +971,13 @@
         <v>25</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.2">
@@ -986,13 +985,13 @@
         <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1000,11 +999,11 @@
         <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="71" x14ac:dyDescent="0.2">
@@ -1012,13 +1011,13 @@
         <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="D12" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
@@ -1026,13 +1025,13 @@
         <v>29</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1040,13 +1039,13 @@
         <v>30</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1070,13 +1069,13 @@
         <v>33</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.2">
@@ -1084,13 +1083,13 @@
         <v>34</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.2">
@@ -1098,10 +1097,10 @@
         <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>13</v>
@@ -1112,13 +1111,13 @@
         <v>36</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="99" x14ac:dyDescent="0.2">
@@ -1132,7 +1131,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.2">
@@ -1140,10 +1139,10 @@
         <v>38</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>8</v>
@@ -1154,13 +1153,13 @@
         <v>39</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1168,13 +1167,13 @@
         <v>40</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
@@ -1182,64 +1181,60 @@
         <v>41</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>70</v>
+      <c r="B27" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="8"/>
+        <v>106</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>46</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D29" s="8"/>
     </row>
@@ -1248,11 +1243,12 @@
         <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D30" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bring in more gis stuff!
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C9A976-5C3E-A14A-BD19-FDFC2F903EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778676FC-7C79-D14C-9A56-469B5DCC5826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="500" windowWidth="32340" windowHeight="19520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -432,8 +432,9 @@
   <si>
     <t>- `What is GIS? &lt;gis_what_is_gis.ipynb&gt;`_
 - `Installing Geopandas &lt;gis_setup_geopandas.ipynb&gt;`_
-- `Geopandas / Vector Data &lt;gis_geopandas.ipynb&gt;`_
-- `GeoPandas User Guide: Data Structures, Reading and Writing Files, and Indexing and Selecting Data &lt;https://geopandas.org/docs/user_guide.html&gt;`_
+- `Geopandas &lt;gis_geopandas.ipynb&gt;`_
+- `Merging Data with Geopandas &lt;gis_relating_data.ipynb&gt;`_
+- `Geospatial Data Formats &lt;gis_data_formats.ipynb&gt;`_
 - **OPIOID PROJECT DUE NOV 21st at 11:59pm (Extensions available upon request to assigned date for PDS final)**</t>
   </si>
 </sst>
@@ -845,7 +846,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1212,7 +1213,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Sarah's first round of edits
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4630F5F-E2C7-674D-AC50-31D06F640BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BDBF39-F13E-7844-BC55-E541AE58BA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="500" windowWidth="32340" windowHeight="19520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -356,10 +356,6 @@
 - `Editing Values &lt;cleaning_editingvalues.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `Git and Github &lt;git_and_github.ipynb&gt;`_
-- `Homework Guidelines &lt;homework_guidelines.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `Principles of Data Visualization &lt;https://www.youtube.com/watch?v=vTingdk_pVM&gt;`_
 - `Intro to Altair &lt;plotting_altair_part1.ipynb&gt;`_
 - `Altair in Context &lt;plotting_altair_in_context.ipynb&gt;`_</t>
@@ -438,6 +434,11 @@
 - `Managing Projections in Geopandas &lt;gis_crs_geopandas.ipynb&gt;`_
 - `Mapping with Python &lt;gis_mapping.ipynb&gt;`_
 **EXERCISE OPTIONAL**</t>
+  </si>
+  <si>
+    <t>- `Git and Github &lt;git_and_github.ipynb&gt;`_
+- `Visualize Git Branches &lt;https://learngitbranching.js.org/&gt;`_
+- `Homework Guidelines &lt;homework_guidelines.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -847,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -983,7 +984,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>26</v>
       </c>
@@ -991,7 +992,7 @@
         <v>61</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>76</v>
@@ -1031,7 +1032,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>71</v>
@@ -1045,10 +1046,10 @@
         <v>52</v>
       </c>
       <c r="C14" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1100,10 +1101,10 @@
         <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>98</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>13</v>
@@ -1145,7 +1146,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>8</v>
@@ -1159,7 +1160,7 @@
         <v>65</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>80</v>
@@ -1184,10 +1185,10 @@
         <v>41</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>82</v>
@@ -1198,7 +1199,7 @@
         <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.2">
@@ -1209,7 +1210,7 @@
         <v>17</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>83</v>
@@ -1223,10 +1224,10 @@
         <v>67</v>
       </c>
       <c r="C28" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1234,13 +1235,13 @@
         <v>46</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
try and push debuggin
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A44559-A658-3045-88EB-69ECA82C80B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE7DBCB-F267-1044-ADA8-3EDDDDC50818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="500" windowWidth="32820" windowHeight="19420" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="9660" yWindow="500" windowWidth="31300" windowHeight="20140" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
 - Distributed Computing</t>
   </si>
   <si>
-    <t>FALL BREAK</t>
-  </si>
-  <si>
     <t>- Advanced Plotting</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
 - LAST CLASS</t>
   </si>
   <si>
-    <t>More time on defining classes</t>
-  </si>
-  <si>
     <t>- `What is GIS? &lt;gis_what_is_gis.ipynb&gt;`_
 - `Installing Geopandas &lt;gis_setup_geopandas.ipynb&gt;`_
 - `Geopandas &lt;gis_geopandas.ipynb&gt;`_
@@ -292,15 +286,6 @@
 - `VS Code Livesharing (first half) &lt;https://www.youtube.com/watch?v=2CTi9THB0b4&gt;`_</t>
   </si>
   <si>
-    <t>- `What are Tracebacks? &lt;https://www.youtube.com/watch?v=JD8BrXXNtjA&gt;`_
-- `Identifying Problems &lt;cleaning_identifying.ipynb&gt;`_
-- `Editing Values Globally &lt;cleaning_editing_globally.ipynb&gt;`_
-- `Editing Locations &lt;cleaning_editing_specific_locations.ipynb&gt;`_
-- `Cleaning Data Types &lt;cleaning_datatypes.ipynb&gt;`_
-- `Missing Data &lt;cleaning_missing_data.ipynb&gt;`_
-- `Python Strings (string section only!) &lt;https://realpython.com/python-data-types/#strings&gt;`_</t>
-  </si>
-  <si>
     <t>Tues, Aug 30</t>
   </si>
   <si>
@@ -338,9 +323,6 @@
   </si>
   <si>
     <t>Thurs, Oct 6</t>
-  </si>
-  <si>
-    <t>Tues, Oct 11</t>
   </si>
   <si>
     <t>Thurs, Oct 13</t>
@@ -416,11 +398,6 @@
 - Packages</t>
   </si>
   <si>
-    <t>- `Python Debugger in VS Code &lt;debugger_vscode.ipynb&gt;`_
-- `variables v objects &lt;vars_v_objects.ipynb&gt;`_
-- `Python v. R &lt;https://www.practicaldatascience.org/html/python_v_r.html&gt;`_</t>
-  </si>
-  <si>
     <t>- **SETUP 1:** `Installing Python and miniconda &lt;setup_python.ipynb&gt;`_
 - **SETUP 2:** `Installing and Configuring VS Code &lt;setup_vscode.ipynb&gt;`_</t>
   </si>
@@ -437,11 +414,43 @@
 - `Python packages &lt;managing_python_packages.ipynb&gt;`_</t>
   </si>
   <si>
+    <t>- `Identifying Problems &lt;cleaning_identifying.ipynb&gt;`_
+- `Editing Values Globally &lt;cleaning_editing_globally.ipynb&gt;`_
+- `Editing Locations &lt;cleaning_editing_specific_locations.ipynb&gt;`_
+- `Cleaning Data Types &lt;cleaning_datatypes.ipynb&gt;`_
+- `Missing Data &lt;cleaning_missing_data.ipynb&gt;`_
+- `Python Strings (string section only!) &lt;https://realpython.com/python-data-types/#strings&gt;`_</t>
+  </si>
+  <si>
     <t>- `Why numpy? &lt;10_why_numpy.ipynb&gt;`_
-- JVP pp 33-77
-- IF did not complete DataCamp: Do Numpy Section
+- `Numpy Vectors &lt;20_vectors.ipynb&gt;`_
+- `Math with Vectors &lt;21_math_with_vectors.ipynb&gt;`_
+- `Subsetting Vectors &lt;30_subsetting_vectors.ipynb&gt;`_
+- `Modifying Subsets of Vectors &lt;35_modifying_subsets_of_vectors.ipynb&gt;`_
 - `Numbers in Computer &lt;ints_and_floats.ipynb&gt;`_
 - `OPTIONAL: How numpy works &lt;https://www.nature.com/articles/s41586-020-2649-2&gt;`_</t>
+  </si>
+  <si>
+    <t>- Numpy Arrays</t>
+  </si>
+  <si>
+    <t>Tues, Oct 11
+**FALL BREAK**</t>
+  </si>
+  <si>
+    <t>- `Views and Copies &lt;10_views_and_copies.ipynb&gt;`_
+- `Matrices &lt;20_matrices.ipynb&gt;`_
+- `Reshaping Matrices &lt;22_reshaping_matrices.ipynb&gt;`_
+- `Images as Matrices &lt;25_images_as_matrices.ipynb&gt;`_
+- `Subsetting Matrices &lt;30_subsetting_matrices.ipynb&gt;`_
+- `ND-Arrays &lt;40_nd_arrays.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `What are Tracebacks? &lt;https://www.youtube.com/watch?v=JD8BrXXNtjA&gt;`_
+- `Debugging Tools &lt;debugger_principles.ipynb&gt;`_
+- `Python Debugger in VS Code &lt;debugger_in_vscode.ipynb&gt;`_
+- `variables v objects &lt;vars_v_objects.ipynb&gt;`_
+- `Python v. R &lt;https://www.practicaldatascience.org/html/python_v_r.html&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -512,9 +521,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -533,6 +539,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -851,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -859,7 +868,7 @@
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="105.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="105.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="57.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -879,33 +888,33 @@
     </row>
     <row r="2" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="9"/>
+        <v>100</v>
+      </c>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>107</v>
+        <v>67</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>9</v>
@@ -916,344 +925,344 @@
     </row>
     <row r="5" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" ht="99" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="71" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="71" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="D14" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="71" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="7" t="s">
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="43" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="C19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="10" t="s">
+      <c r="C21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="99" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+    <row r="22" spans="1:4" ht="99" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="B22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="13" t="s">
+      <c r="B23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="99" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+      <c r="C26" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
+      <c r="D27" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B28" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
+      <c r="C28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
+      <c r="B29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="9" t="s">
+      <c r="C30" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update debugger exercise links
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CDADB1B7-5481-9048-A8D5-DD3D822FD76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4463F5F8-AC7F-CC4E-ADEB-BF66FCF9E971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7100" yWindow="500" windowWidth="31300" windowHeight="19420" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -867,7 +867,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
push new exercise links
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5D3EC6-A20D-164C-8D05-D71D496598F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E533B2B-7591-CE40-9336-1291EFFD7A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="31300" windowHeight="19420" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Topic</t>
   </si>
@@ -458,6 +458,9 @@
 - `Modifying Subsets of Vectors &lt;35_modifying_subsets_of_vectors.ipynb&gt;`_
 - `Numbers in Computer &lt;ints_and_floats.ipynb&gt;`_
 - `Wanna leave feedback? &lt;https://forms.gle/KUcCX2vjE3Jqb4EN9&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Ex 1 &lt;https://github.com/nickeubank/practicaldatascience/raw/master/source/exercises/numpy_vectors.ipynb.zip&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -868,7 +871,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,6 +971,9 @@
       <c r="C7" s="3" t="s">
         <v>110</v>
       </c>
+      <c r="D7" s="8" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">

</xml_diff>

<commit_message>
update pandas week 1
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E533B2B-7591-CE40-9336-1291EFFD7A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EF1EF1-8538-FF4F-BD0E-7FF327D302CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="31300" windowHeight="19420" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="8800" yWindow="500" windowWidth="31300" windowHeight="19420" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>In-Class Exercise</t>
   </si>
   <si>
-    <t>- `Pandas 1: Series &lt;pandas_series.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `Pandas 2: DataFrames &lt;pandas_dataframes.ipynb&gt;`_</t>
   </si>
   <si>
@@ -461,6 +458,12 @@
   </si>
   <si>
     <t>- `Ex 1 &lt;https://github.com/nickeubank/practicaldatascience/raw/master/source/exercises/numpy_vectors.ipynb.zip&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Broadcasting in numpy &lt;41_broadcasting.ipynb&gt;`_
+- `Why Pandas? &lt;00_intro_to_pandas.ipynb&gt;`_
+- `Pandas Series &lt;10_pandas_series.ipynb&gt;`_
+- `Manipulating Pandas Series &lt;15_manipulating_series.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -871,7 +874,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -884,7 +887,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -898,386 +901,386 @@
     </row>
     <row r="2" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>53</v>
-      </c>
       <c r="D20" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="99" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="D26" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ad vectorization and update series exercises
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EF1EF1-8538-FF4F-BD0E-7FF327D302CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1554DB5-5C9A-AD4C-8D15-22A3B3200F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8800" yWindow="500" windowWidth="31300" windowHeight="19420" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -463,7 +463,8 @@
     <t>- `Broadcasting in numpy &lt;41_broadcasting.ipynb&gt;`_
 - `Why Pandas? &lt;00_intro_to_pandas.ipynb&gt;`_
 - `Pandas Series &lt;10_pandas_series.ipynb&gt;`_
-- `Manipulating Pandas Series &lt;15_manipulating_series.ipynb&gt;`_</t>
+- `Manipulating Pandas Series &lt;15_manipulating_series.ipynb&gt;`_
+- `Vectorizing &lt;11_vectorization.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -992,7 +993,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
update schedule and add section numbers
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3F8F7C-AC99-9046-83B6-3C58BAFCE4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487C17A8-1B2E-2B4C-ABE3-0E43E86A1C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8800" yWindow="500" windowWidth="31300" windowHeight="19420" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -457,14 +457,14 @@
 - `Writing Good Notebooks &lt;writing_good_jupyter_notebooks.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- WM pp 136-142 (Indices)
-- JVP pp 115-139 (Missing Data)
+    <t>- `Git and Github &lt;git_and_github.ipynb&gt;`_
+- `Visualize Git Branches &lt;https://learngitbranching.js.org/&gt;`_</t>
+  </si>
+  <si>
+    <t>- WM pp 136-142 (Indices, Section 5.2 up to MultiIndexes)
+- JVP pp 119-127 ("Handling Missing Data" in Chpt 3)
 - `Views and Copies in Numpy &lt;views_and_copies_numpy_review.ipynb&gt;`_
 - `Views and Copies in Pandas &lt;views_and_copies_in_pandas.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Git and Github &lt;git_and_github.ipynb&gt;`_
-- `Visualize Git Branches &lt;https://learngitbranching.js.org/&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -875,7 +875,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,7 +1029,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>32</v>
@@ -1043,7 +1043,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
first half reorg for 2023, no html
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E50243C-34AE-454E-9128-35DD88FA5B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D5ECA2-A355-F342-9E8F-592650C41984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="1540" windowWidth="30240" windowHeight="17200" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="6860" yWindow="500" windowWidth="30240" windowHeight="17200" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -282,14 +282,6 @@
 - Welcome to VS Code</t>
   </si>
   <si>
-    <t xml:space="preserve">- **SETUP 3:** `Setup Augmented Command Line &lt;setup_augmented_commandline.ipynb&gt;`_
-- `Command Line Basics &lt;command_line_part1.ipynb&gt;`_
-- `Read and sign syllabus &lt;https://github.com/nickeubank/practicaldatascience/raw/master/syllabus/Syllabus_PracticalDataScience.pdf&gt;`_
-- `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
-- `Register for DataCamp &lt;https://www.datacamp.com/home&gt;`_
-</t>
-  </si>
-  <si>
     <t>- Command Line Basics</t>
   </si>
   <si>
@@ -303,10 +295,6 @@
 - Packages</t>
   </si>
   <si>
-    <t>- **SETUP 1:** `Installing Python and miniconda &lt;setup_python.ipynb&gt;`_
-- **SETUP 2:** `Installing and Configuring VS Code &lt;setup_vscode.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `Ex 1 &lt;exercises/Exercise_CommandLine_2_Advanced.ipynb&gt;`_
 - `Ex 2 &lt;exercises/Exercise_jupytervscode.ipynb&gt;`_</t>
   </si>
@@ -321,49 +309,15 @@
 **FALL BREAK**</t>
   </si>
   <si>
-    <t>- `What are Tracebacks? &lt;https://www.youtube.com/watch?v=JD8BrXXNtjA&gt;`_
-- `Debugging Tools &lt;debugging_principles.ipynb&gt;`_
-- `Python Debugger in VS Code &lt;debugging_in_vscode.ipynb&gt;`_
-- `variables v objects &lt;vars_v_objects.ipynb&gt;`_
-- `Python v. R &lt;https://www.practicaldatascience.org/html/python_v_r.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Advanced Command Line &lt;command_line_part2.ipynb&gt;`_
-- **SETUP 4:** `Jupyter in VS Code &lt;jupyter.ipynb&gt;`_
-- `Python packages &lt;managing_python_packages.ipynb&gt;`_
-- **OPTIONAL SETUP:** `R Notebooks &lt;jupyter_r_notebooks.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `Ex 1 &lt;exercises/Exercise_debugger.ipynb&gt;`_
 - `Ex 2 &lt;exercises/Exercise_variables_v_objects.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `Why numpy? &lt;10_why_numpy.ipynb&gt;`_
-- `Numpy Vectors &lt;20_intro_to_vectors.ipynb&gt;`_
-- `Math with Vectors &lt;21_math_with_vectors.ipynb&gt;`_
-- `Type Promotion &lt;23_type_promotion_in_vectors.ipynb&gt;`_
-- `Subsetting Vectors &lt;30_subsetting_vectors.ipynb&gt;`_
-- `Modifying Subsets of Vectors &lt;35_modifying_subsets_of_vectors.ipynb&gt;`_
-- `Numbers in Computer &lt;ints_and_floats.ipynb&gt;`_
-- `Wanna leave feedback? &lt;https://forms.gle/KUcCX2vjE3Jqb4EN9&gt;`_</t>
-  </si>
-  <si>
     <t>- `Ex 1 &lt;https://github.com/nickeubank/practicaldatascience/raw/master/source/exercises/numpy_vectors.ipynb.zip&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Pandas 2: DataFrames &lt;30_pandas_dataframes.ipynb&gt;`_
-- `Managing Settings in VS Code &lt;https://youtu.be/Knc6S4gUHzk&gt;`_
-- `Writing Good Notebooks &lt;writing_good_jupyter_notebooks.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- `Git and Github &lt;git_and_github.ipynb&gt;`_
 - `Visualize Git Branches &lt;https://learngitbranching.js.org/&gt;`_</t>
-  </si>
-  <si>
-    <t>- WM pp 136-142 (Indices, Section 5.2 up to MultiIndexes)
-- JVP pp 119-127 ("Handling Missing Data" in Chpt 3)
-- `Views and Copies in Numpy &lt;views_and_copies_numpy_review.ipynb&gt;`_
-- `Views and Copies in Pandas &lt;views_and_copies_in_pandas.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- Oopsie Resource: `Oh 💩, Git! &lt;https://ohshitgit.com/&gt;`_
@@ -374,22 +328,6 @@
 - `Intro to Altair &lt;plotting_altair_part1.ipynb&gt;`_
 - `Altair in Context &lt;plotting_altair_in_context.ipynb&gt;`_
 - `Plotting with Pandas &lt;plotting_with_pandas.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Why Pandas? &lt;00_intro_to_pandas.ipynb&gt;`_
-- `Pandas Series &lt;10_pandas_series.ipynb&gt;`_
-- `Manipulating Pandas Series &lt;15_manipulating_series.ipynb&gt;`_
-- `Vectorizing &lt;11_vectorization.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Views and Copies &lt;10_views_and_copies.ipynb&gt;`_
-- `Matrices &lt;20_matrices.ipynb&gt;`_
-- `Reshaping Matrices &lt;22_reshaping_matrices.ipynb&gt;`_
-- `Images as Matrices &lt;25_images_as_matrices.ipynb&gt;`_
-- `Subsetting Matrices &lt;30_subsetting_matrices.ipynb&gt;`_
-- `ND-Arrays &lt;40_nd_arrays.ipynb&gt;`_
-- `Broadcasting in numpy &lt;41_broadcasting.ipynb&gt;`_
-- `Wanna leave some feedback? &lt;https://forms.gle/s5PknVTvqzPJtCu49&gt;`_</t>
   </si>
   <si>
     <t>- Defensive Programming
@@ -455,6 +393,80 @@
 (Note reading includes a 45 minute video to watch)
 **Optional:**
 - `Setting Up Cloud Cluster &lt;distributed_starting_dask_cluster.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- **SETUP 1:** `Installing Python and miniconda &lt;00_setup_env/setup_python.ipynb&gt;`_
+- **SETUP 2:** `Installing and Configuring VS Code &lt;00_setup_env/setup_vscode.ipynb&gt;`_
+- `chatGPT and You &lt;llms.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- **SETUP 3:** `Setup Augmented Command Line &lt;00_setup_env/setup_augmented_commandline.ipynb&gt;`_
+- `Command Line Basics &lt;10_commandline/commandline_part1.ipynb&gt;`_
+- `Read and sign syllabus &lt;https://github.com/nickeubank/practicaldatascience/raw/master/syllabus/Syllabus_PracticalDataScience.pdf&gt;`_
+- `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
+- `Register for DataCamp &lt;https://www.datacamp.com/home&gt;`_
+</t>
+  </si>
+  <si>
+    <t>- `Advanced Command Line &lt;10_commandline/commandline_part2.ipynb&gt;`_
+- **SETUP 4:** `Jupyter in VS Code &lt;00_setup_env/jupyter_in_vscode.ipynb&gt;`_
+- `Python packages &lt;00_setup_env/managing_python_packages.ipynb&gt;`_
+- **OPTIONAL SETUP:** `R Notebooks &lt;00_setup_env/jupyter_r_notebooks.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `What are Tracebacks? &lt;https://www.youtube.com/watch?v=JD8BrXXNtjA&gt;`_
+- `Debugging Tools &lt;20_programming_skills/10_debugging_principles.ipynb&gt;`_
+- `Python Debugger in VS Code &lt;20_programming_skills/20_debugging_in_vscode.ipynb&gt;`_
+- `variables v objects &lt;misc/vars_v_objects.ipynb&gt;`_
+- `Python v. R &lt;misc/python_v_r.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Why numpy? &lt;30_numpy/10_vectors/10_why_numpy.ipynb&gt;`_
+- `Numpy Vectors &lt;30_numpy/10_vectors/20_intro_to_vectors.ipynb&gt;`_
+- `Math with Vectors &lt;30_numpy/10_vectors/21_math_with_vectors.ipynb&gt;`_
+- `Type Promotion &lt;30_numpy/10_vectors/23_type_promotion_in_vectors.ipynb&gt;`_
+- `Vector Recap &lt;30_numpy/10_vectors/24_vector_recap.ipynb&gt;`_
+- `Subsetting Vectors &lt;30_numpy/10_vectors/30_subsetting_vectors.ipynb&gt;`_
+- `Modifying Subsets of Vectors &lt;30_numpy/10_vectors/35_modifying_subsets_of_vectors.ipynb&gt;`_
+- `Vector Subsetting Recap &lt;30_numpy/10_vectors/37_vector_subsets_recap.ipynb&gt;`_
+- `Numbers in Computer &lt;20_programming_skills/ints_and_floats.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>**More Numpy Concepts:**
+- `Views and Copies &lt;30_numpy/15_advanced_numpy_concepts/10_views_and_copies.ipynb&gt;`_
+- `When Do I Get a View &lt;30_numpy/15_advanced_numpy_concepts/11_when_do_I_get_a_view.ipynb&gt;`_
+- `Views and Copies Recap &lt;30_numpy/15_advanced_numpy_concepts/12_views_and_copies_recap.ipynb&gt;`_
+- `Objects and Variables &lt;30_numpy/15_advanced_numpy_concepts/13_objects_and_variables.ipynb&gt;`_
+**Matrices:**
+- `Welcome to Matrices &lt;30_numpy/20_matrices/00_welcome_to_matrices.ipynb&gt;`_
+- `Matrices &lt;30_numpy/20_matrices/20_matrices.ipynb&gt;`_
+- `Reshaping Matrices &lt;30_numpy/20_matrices/22_reshaping_matrices.ipynb&gt;`_
+- `Images as Matrices &lt;30_numpy/20_matrices/25_images_as_matrices.ipynb&gt;`_
+- `Subsetting Matrices &lt;30_numpy/20_matrices/30_subsetting_matrices.ipynb&gt;`_
+- `Matrices Recap &lt;30_numpy/20_matrices/33_matrix_recaps.ipynb&gt;
+**ND Arrays:**
+- `ND-Arrays &lt;30_numpy/20_matrices/40_nd_arrays.ipynb&gt;`_
+- `Broadcasting in numpy &lt;30_numpy/20_matrices/41_broadcasting.ipynb&gt;`_
+- `ND Array Recap &lt;30_numpy/20_matrices/42_nd_array_review.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Why Pandas? &lt;40_pandas_basics/00_intro_to_pandas.ipynb&gt;`_
+- `Pandas Series &lt;40_pandas_basics/10_pandas_series.ipynb&gt;`_
+- `Manipulating Pandas Series &lt;40_pandas_basics/15_manipulating_series.ipynb&gt;`_
+- `Vectorization &lt;30_numpy/40_advanced_numpy/11_vectorization.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Pandas DataFrames &lt;40_pandas_basics/30_pandas_dataframes.ipynb&gt;`_
+- `Pandas DataFrame Gotchas &lt;40_pandas_basics/35_pandas_dataframe_gotchas.ipynb&gt;`_
+- `Managing Settings in VS Code &lt;https://youtu.be/Knc6S4gUHzk&gt;`_
+- `Writing Good Notebooks &lt;20_programming_skills/writing_good_jupyter_notebooks.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- WM pp 136-142 (Indices, Section 5.2 up to MultiIndexes)
+- JVP pp 119-127 ("Handling Missing Data" in Chpt 3)
+- `Numpy Views and Copies Review &lt;40_pandas_basics/10_views_and_copies_numpy_review.ipynb&gt;`_
+- `Views and Copies in Pandas &lt;40_pandas_basics/50_views_and_copies_in_pandas.ipynb&gt;`_
+- `Views and Copies in Pandas W/O CoW &lt;40_pandas_basics/50_views_and_copies_in_pandas_wo_CoW.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -515,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -535,9 +547,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -861,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -895,7 +904,7 @@
         <v>74</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="D2" s="8"/>
     </row>
@@ -903,14 +912,14 @@
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>75</v>
       </c>
+      <c r="C3" s="12" t="s">
+        <v>102</v>
+      </c>
       <c r="D3" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -929,13 +938,13 @@
         <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -943,16 +952,16 @@
         <v>50</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>84</v>
+        <v>76</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="113" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="127" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>51</v>
       </c>
@@ -960,21 +969,21 @@
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="356" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>95</v>
+        <v>80</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>24</v>
@@ -988,7 +997,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>25</v>
@@ -1002,13 +1011,13 @@
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>55</v>
       </c>
@@ -1016,7 +1025,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>28</v>
@@ -1030,7 +1039,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>32</v>
@@ -1044,7 +1053,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>33</v>
@@ -1058,15 +1067,15 @@
         <v>39</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
-        <v>83</v>
+      <c r="A15" s="13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1082,7 +1091,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>27</v>
@@ -1092,13 +1101,13 @@
       <c r="A18" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1137,8 +1146,8 @@
       <c r="B21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>97</v>
+      <c r="C21" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>8</v>
@@ -1149,10 +1158,10 @@
         <v>65</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>34</v>
@@ -1194,7 +1203,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>36</v>
@@ -1208,10 +1217,10 @@
         <v>23</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1219,7 +1228,7 @@
         <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1238,7 +1247,7 @@
         <v>44</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>37</v>
@@ -1246,27 +1255,28 @@
     </row>
     <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
thin out local content
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3E6A06-E271-894F-8575-3C81EDAAA751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567CD7C6-9008-E241-B0AD-3D683AAE735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6860" yWindow="500" windowWidth="30240" windowHeight="17200" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -385,25 +385,6 @@
 - `Setting Up Cloud Cluster &lt;distributed_starting_dask_cluster.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- **SETUP 1:** `Installing Python and miniconda &lt;00_setup_env/setup_python.ipynb&gt;`_
-- **SETUP 2:** `Installing and Configuring VS Code &lt;00_setup_env/setup_vscode.ipynb&gt;`_
-- `chatGPT and You &lt;llms.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- **SETUP 3:** `Setup Augmented Command Line &lt;00_setup_env/setup_augmented_commandline.ipynb&gt;`_
-- `Command Line Basics &lt;10_commandline/commandline_part1.ipynb&gt;`_
-- `Read and sign syllabus &lt;https://github.com/nickeubank/practicaldatascience/raw/master/syllabus/Syllabus_PracticalDataScience.pdf&gt;`_
-- `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
-- `Register for DataCamp &lt;https://www.datacamp.com/home&gt;`_
-</t>
-  </si>
-  <si>
-    <t>- `Advanced Command Line &lt;10_commandline/commandline_part2.ipynb&gt;`_
-- **SETUP 4:** `Jupyter in VS Code &lt;00_setup_env/jupyter_in_vscode.ipynb&gt;`_
-- `Python packages &lt;00_setup_env/managing_python_packages.ipynb&gt;`_
-- **OPTIONAL SETUP:** `R Notebooks &lt;00_setup_env/jupyter_r_notebooks.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `Why numpy? &lt;30_numpy/10_vectors/10_why_numpy.ipynb&gt;`_
 - `Numpy Vectors &lt;30_numpy/10_vectors/20_intro_to_vectors.ipynb&gt;`_
 - `Math with Vectors &lt;30_numpy/10_vectors/21_math_with_vectors.ipynb&gt;`_
@@ -452,13 +433,6 @@
 - `Views and Copies in Pandas W/O CoW &lt;40_pandas_basics/50_views_and_copies_in_pandas_wo_CoW.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `What are Tracebacks? &lt;https://www.youtube.com/watch?v=JD8BrXXNtjA&gt;`_
-- `Debugging Tools &lt;20_programming_concepts/10_debugging_principles.ipynb&gt;`_
-- `Python Debugger in VS Code &lt;20_programming_concepts/20_debugging_in_vscode.ipynb&gt;`_
-- `variables v objects &lt;misc/vars_v_objects.ipynb&gt;`_
-- `Python v. R &lt;misc/python_v_r.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `Defensive Programming &lt;20_programming_concepts/defensive_programming.ipynb&gt;`_
 - `Iceberg Principle &lt;20_programming_concepts/iceberg_principle.ipynb&gt;`_
 - WM pp Chpt 10, 10.1, 10.2, 10.3</t>
@@ -467,6 +441,32 @@
     <t>- `Workflow Management &lt;20_programming_concepts/workflow.ipynb&gt;`_
 - `Backwards Design &lt;20_programming_concepts/backwards_design.ipynb&gt;`_
 - `Getting Help &lt;20_programming_concepts/getting_help.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- **SETUP 1:** `Installing Python and miniconda &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_python.html&gt;`_
+- **SETUP 2:** `Installing and Configuring VS Code &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_vscode.html&gt;`_
+- `chatGPT and You &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/99_advice/llms.html&gt;`_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- **SETUP 3:** `Setup Augmented Command Line &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_augmented_commandline.html&gt;`_
+- `Command Line Basics &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/10_commandline/commandline_part1.html&gt;`_
+- `Read and sign syllabus &lt;https://github.com/nickeubank/practicaldatascience/raw/master/syllabus/Syllabus_PracticalDataScience.pdf&gt;`_
+- `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
+- `Register for DataCamp &lt;https://www.datacamp.com/home&gt;`_
+</t>
+  </si>
+  <si>
+    <t>- `Advanced Command Line &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/10_commandline/commandline_part2.html&gt;`_
+- **SETUP 4:** `Jupyter in VS Code &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/00_setup_env/jupyter_in_vscode.html&gt;`_
+- `Python packages &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/class_2/week_4/30_managing_python_packages.html&gt;`_
+- **OPTIONAL SETUP:** `R Jupyter Notebooks &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/00_setup_env/jupyter_r_notebooks.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `What are Tracebacks? &lt;https://www.youtube.com/watch?v=JD8BrXXNtjA&gt;`_
+- `Debugging Tools &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/10_debugging_principles.html&gt;`_
+- `Python Debugger in VS Code &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/20_debugging_in_vscode.html&gt;`_
+- `variables v objects &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/vars_v_objects.html&gt;`_
+- `Python v. R &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/python_v_r.html&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -904,7 +904,7 @@
         <v>74</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D2" s="8"/>
     </row>
@@ -916,7 +916,7 @@
         <v>75</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>79</v>
@@ -933,7 +933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="155" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -941,13 +941,13 @@
         <v>77</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="221" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
@@ -955,7 +955,7 @@
         <v>76</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>82</v>
@@ -969,7 +969,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>83</v>
@@ -983,7 +983,7 @@
         <v>80</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>24</v>
@@ -997,7 +997,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>25</v>
@@ -1011,7 +1011,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>26</v>
@@ -1025,7 +1025,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>28</v>
@@ -1147,7 +1147,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>8</v>
@@ -1161,7 +1161,7 @@
         <v>87</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
add chat gpt to syllabus signatures
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567CD7C6-9008-E241-B0AD-3D683AAE735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFDDADC-ED87-0B4A-A8ED-E64227DF2353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6860" yWindow="500" windowWidth="30240" windowHeight="17200" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
   <si>
     <t>Topic</t>
   </si>
@@ -194,87 +194,6 @@
 - `Code Reviews &lt;pr_review.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>Tues, Aug 30</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 1</t>
-  </si>
-  <si>
-    <t>Fri, Sep 2</t>
-  </si>
-  <si>
-    <t>Tues, Sep 6</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 8</t>
-  </si>
-  <si>
-    <t>Tues, Sep 13</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 15</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 22</t>
-  </si>
-  <si>
-    <t>Tues, Sep 20</t>
-  </si>
-  <si>
-    <t>Tues, Sep 27</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 29</t>
-  </si>
-  <si>
-    <t>Tues, Oct 4</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 6</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 13</t>
-  </si>
-  <si>
-    <t>Tues, Oct 18</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 20</t>
-  </si>
-  <si>
-    <t>Tues, Oct 25</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 27</t>
-  </si>
-  <si>
-    <t>Tues, Nov 1</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 3</t>
-  </si>
-  <si>
-    <t>Tues, Nov 8</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 10</t>
-  </si>
-  <si>
-    <t>Tues, Nov 15</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 17</t>
-  </si>
-  <si>
-    <t>Tues, Nov 22</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 24</t>
-  </si>
-  <si>
-    <t>Tues, Nov 29</t>
-  </si>
-  <si>
     <t>THANKSGIVING</t>
   </si>
   <si>
@@ -303,10 +222,6 @@
   </si>
   <si>
     <t>- Numpy Arrays</t>
-  </si>
-  <si>
-    <t>Tues, Oct 11
-**FALL BREAK**</t>
   </si>
   <si>
     <t>- `Ex 1 &lt;exercises/Exercise_debugger.ipynb&gt;`_
@@ -340,12 +255,6 @@
 - `Cleaning Data Types &lt;33_cleaning_datatypes.ipynb&gt;`_
 - `Missing Data &lt;35_cleaning_missing_data.ipynb&gt;`_
 - `Python Strings (string section only!) &lt;https://realpython.com/python-data-types/#strings&gt;`_</t>
-  </si>
-  <si>
-    <t>Thurs, Dec 1</t>
-  </si>
-  <si>
-    <t>Fri, Dec 9th</t>
   </si>
   <si>
     <t>**Final Project Report and Presentation Due**</t>
@@ -467,6 +376,99 @@
 - `Python Debugger in VS Code &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/20_debugging_in_vscode.html&gt;`_
 - `variables v objects &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/vars_v_objects.html&gt;`_
 - `Python v. R &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/python_v_r.html&gt;`_</t>
+  </si>
+  <si>
+    <t>Tues, Aug 29</t>
+  </si>
+  <si>
+    <t>Thurs, Aug 31</t>
+  </si>
+  <si>
+    <t>Fri, Sep 1</t>
+  </si>
+  <si>
+    <t>Tues, Sep 5</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 7</t>
+  </si>
+  <si>
+    <t>Tues, Sep 12</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 14</t>
+  </si>
+  <si>
+    <t>Tues, Sep 19</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 21</t>
+  </si>
+  <si>
+    <t>Tues, Sep 26</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 28</t>
+  </si>
+  <si>
+    <t>Tues, Oct 3</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 5</t>
+  </si>
+  <si>
+    <t>**FALL BREAK**</t>
+  </si>
+  <si>
+    <t>Tues, Oct 10</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 12</t>
+  </si>
+  <si>
+    <t>Tues, Oct 17</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 19</t>
+  </si>
+  <si>
+    <t>Tues, Oct 24</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 26</t>
+  </si>
+  <si>
+    <t>Tues, Oct 31</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 2</t>
+  </si>
+  <si>
+    <t>Tues, Nov 7</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 9</t>
+  </si>
+  <si>
+    <t>Tues, Nov 14</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 16</t>
+  </si>
+  <si>
+    <t>Tues, Nov 21</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 23</t>
+  </si>
+  <si>
+    <t>Tues, Nov 28</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 30</t>
+  </si>
+  <si>
+    <t>Fri, Dec 8</t>
   </si>
 </sst>
 </file>
@@ -870,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -898,33 +900,33 @@
     </row>
     <row r="2" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -935,55 +937,55 @@
     </row>
     <row r="5" spans="1:4" ht="155" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="221" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="127" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="356" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>24</v>
@@ -991,13 +993,13 @@
     </row>
     <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>25</v>
@@ -1005,13 +1007,13 @@
     </row>
     <row r="10" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>26</v>
@@ -1019,13 +1021,13 @@
     </row>
     <row r="11" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>28</v>
@@ -1033,13 +1035,13 @@
     </row>
     <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>32</v>
@@ -1047,13 +1049,13 @@
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>33</v>
@@ -1061,45 +1063,51 @@
     </row>
     <row r="14" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>81</v>
+        <v>94</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="B16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>27</v>
+        <v>96</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>12</v>
@@ -1113,7 +1121,7 @@
     </row>
     <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>40</v>
@@ -1127,7 +1135,7 @@
     </row>
     <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>18</v>
@@ -1141,13 +1149,13 @@
     </row>
     <row r="21" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>8</v>
@@ -1155,13 +1163,13 @@
     </row>
     <row r="22" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>34</v>
@@ -1169,7 +1177,7 @@
     </row>
     <row r="23" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>4</v>
@@ -1183,7 +1191,7 @@
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>21</v>
@@ -1197,13 +1205,13 @@
     </row>
     <row r="25" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>36</v>
@@ -1211,43 +1219,43 @@
     </row>
     <row r="26" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>37</v>
@@ -1255,24 +1263,24 @@
     </row>
     <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates of exercise keys and schedule
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FD1FD9-AFBF-8B4F-96BA-F0C928D3ADC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13EC71F-B904-B348-82BA-7229E798AA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -200,9 +200,6 @@
 - `Ex 2 &lt;exercises/Exercise_variables_v_objects.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `Ex 1 &lt;https://github.com/nickeubank/practicaldatascience/raw/master/source/exercises/numpy_vectors.ipynb.zip&gt;`_</t>
-  </si>
-  <si>
     <t>- `Principles of Data Visualization &lt;https://www.youtube.com/watch?v=vTingdk_pVM&gt;`_
 - `Intro to Altair &lt;plotting_altair_part1.ipynb&gt;`_
 - `Altair in Context &lt;plotting_altair_in_context.ipynb&gt;`_
@@ -457,6 +454,9 @@
   </si>
   <si>
     <t>- `Link &lt;exercises/Exercise_plotting_part2.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Ex 1 &lt;exercises/Exercise_numpy_vectors.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,25 +888,25 @@
     </row>
     <row r="2" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>44</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -925,41 +925,41 @@
     </row>
     <row r="5" spans="1:4" ht="99" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="165" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>46</v>
@@ -967,27 +967,27 @@
     </row>
     <row r="8" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="356" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>22</v>
@@ -995,13 +995,13 @@
     </row>
     <row r="10" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>23</v>
@@ -1009,13 +1009,13 @@
     </row>
     <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>24</v>
@@ -1023,13 +1023,13 @@
     </row>
     <row r="12" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>26</v>
@@ -1037,13 +1037,13 @@
     </row>
     <row r="13" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>27</v>
@@ -1051,13 +1051,13 @@
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>25</v>
@@ -1065,34 +1065,34 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>36</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>18</v>
@@ -1120,13 +1120,13 @@
     </row>
     <row r="20" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>8</v>
@@ -1134,13 +1134,13 @@
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>30</v>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="22" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>4</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="23" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>19</v>
@@ -1176,13 +1176,13 @@
     </row>
     <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>32</v>
@@ -1190,34 +1190,34 @@
     </row>
     <row r="25" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
@@ -1225,13 +1225,13 @@
     </row>
     <row r="29" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>33</v>
@@ -1239,24 +1239,24 @@
     </row>
     <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update exercises on class schedule to remove before ready
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2EE880-6A6C-DB4F-B637-29F4980A15FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{20E518D6-B9ED-BB47-943F-B638659E8D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <t>Topic</t>
   </si>
@@ -51,16 +51,10 @@
 - Pandas: Categoricals</t>
   </si>
   <si>
-    <t>[finish groupby and reshaping exercises]</t>
-  </si>
-  <si>
     <t>**SOFTWARE INSTALL DAY**</t>
   </si>
   <si>
     <t>A day of trouble shooting install issues</t>
-  </si>
-  <si>
-    <t>**Discuss mid-semester project in class**</t>
   </si>
   <si>
     <t>- `What is Big Data? &lt;what_is_big_data.ipynb&gt;`_
@@ -112,37 +106,6 @@
   </si>
   <si>
     <t>- `Link &lt;exercises/Exercise_series.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_dataframe.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_plotting_part1.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link 1 &lt;exercises/Exercise_indices.ipynb&gt;`_
-- `Link 2 &lt;exercises/Exercise_missing.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_cleaning.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_merging.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_bigdata.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_groupby.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_reshaping.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_statsmodels.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_codeyourownlinearregression.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- JVP pp 149 - 157
@@ -229,9 +192,6 @@
 - `Patsy: Differences from R &lt;https://patsy.readthedocs.io/en/latest/R-comparison.html&gt;`_</t>
   </si>
   <si>
-    <t>- `Link &lt;exercises/Exercise_sklearn.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- Review linear regression as matrix manipulations. `Here's a nice review. &lt;https://www.stat.purdue.edu/~boli/stat512/lectures/topic3.pdf&gt;`_
 - `Review how to define classes &lt;https://realpython.com/python3-object-oriented-programming/&gt;`_
 - `Broadcasting in numpy &lt;41_broadcasting.ipynb&gt;`_
@@ -239,10 +199,6 @@
   </si>
   <si>
     <t>No Class</t>
-  </si>
-  <si>
-    <t>- `Link 1 &lt;exercises/Exercise_dask_realdata.ipynb&gt;`_
-- `Link 2 &lt;exercises/Exercise_dask.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_
@@ -409,9 +365,6 @@
   <si>
     <t>- Git Continued
 - Jupyter</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/Exercise_plotting_part2.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- `Ex 1 &lt;exercises/Exercise_numpy_vectors.ipynb&gt;`_</t>
@@ -846,7 +799,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -873,375 +826,345 @@
     </row>
     <row r="2" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="99" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="165" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>23</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>25</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>26</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>100</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>27</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>28</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>8</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>29</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>30</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>5</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>31</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>52</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>32</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>55</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with exercies for thurs
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB75585-1842-304E-96C9-28C4D0C53CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F90AF9-C8F4-2640-8829-486935F333C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="3300" yWindow="3840" windowWidth="30240" windowHeight="17520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
   <si>
     <t>Topic</t>
   </si>
@@ -398,6 +398,10 @@
   </si>
   <si>
     <t>- `Link &lt;exercises/Exercise_dataframes.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link 1 &lt;exercises/Exercise_indices.ipynb&gt;`_
+- `Link 2 &lt;exercises/Exercise_missing.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -802,7 +806,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -972,7 +976,9 @@
       <c r="C12" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">

</xml_diff>

<commit_message>
add additional groupby reading
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F052B750-2618-824F-B64A-DFF1E4293733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5894250C-EB49-434F-A8F2-24BBCA1C56D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="30240" windowHeight="17520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -387,11 +387,6 @@
 - `Parquet Format &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/30_big_data/30_parquet.html&gt;`_</t>
   </si>
   <si>
-    <t>- `Defensive Programming &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/defensive_programming.html&gt;`_
-- `Iceberg Principle &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/iceberg_principle.html&gt;`_
-- `Groupby &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/class_3/week_4/20_grouping.html&gt;`_</t>
-  </si>
-  <si>
     <t>- `Ex &lt;exercises/Exercise_bigdata.ipynb&gt;`_</t>
   </si>
   <si>
@@ -411,6 +406,12 @@
 - `Improving Performance &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/30_big_data/50_performance_solutions.html&gt;`_
 - `Code Reviews &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/pr_review.html&gt;`_
 - **Project Strategy Plan Due**</t>
+  </si>
+  <si>
+    <t>- `Defensive Programming &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/defensive_programming.html&gt;`_
+- `Iceberg Principle &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/iceberg_principle.html&gt;`_
+- `Groupby &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/class_3/week_4/20_grouping.html&gt;`_
+- WM pp Chpt 10, 10.1, 10.2, 10.3</t>
   </si>
 </sst>
 </file>
@@ -815,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1073,7 +1074,7 @@
         <v>93</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="105" x14ac:dyDescent="0.2">
@@ -1084,11 +1085,11 @@
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" ht="90" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>57</v>
       </c>
@@ -1096,7 +1097,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D21" s="9"/>
     </row>
@@ -1108,7 +1109,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="8"/>
     </row>
@@ -1120,7 +1121,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="7"/>
     </row>

</xml_diff>

<commit_message>
update groupby and reshapeing
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5894250C-EB49-434F-A8F2-24BBCA1C56D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F217742-1EF8-F346-BE7A-DA5E31908564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="30240" windowHeight="17520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -396,12 +396,6 @@
 - `Opioid Project &lt;https://github.com/nickeubank/practicaldatascience/blob/master/opioid_project/PDS_ProjectSummary.pdf&gt;`_</t>
   </si>
   <si>
-    <t>- WM 8.3
-- `Pandas reshaping (with pics!) &lt;https://pandas.pydata.org/pandas-docs/stable/user_guide/reshaping.html&gt;`_
-- `What is goal of reshaping? &lt;https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;ved=2ahUKEwifqfmGn6_sAhWfgnIEHQo2AwAQFjACegQIAxAC&amp;url=https%3A%2F%2Fvita.had.co.nz%2Fpapers%2Ftidy-data.pdf&amp;usg=AOvVaw3HDG0hKNeQpAOVcdczJizw&gt;`_
-- Categoricals: WM 12.1</t>
-  </si>
-  <si>
     <t>- `Understanding Performance &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/30_big_data/40_performance_understanding.html&gt;`_
 - `Improving Performance &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/30_big_data/50_performance_solutions.html&gt;`_
 - `Code Reviews &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/pr_review.html&gt;`_
@@ -412,6 +406,12 @@
 - `Iceberg Principle &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/PDS_not_yet_in_coursera/20_programming_concepts/iceberg_principle.html&gt;`_
 - `Groupby &lt;https://nickeubank.github.io/practicaldatascience_book/notebooks/class_3/week_4/20_grouping.html&gt;`_
 - WM pp Chpt 10, 10.1, 10.2, 10.3</t>
+  </si>
+  <si>
+    <t>- WM 8.3
+- `Pandas reshaping (with pics!) &lt;https://pandas.pydata.org/pandas-docs/stable/user_guide/reshaping.html&gt;`_
+- `What is goal of reshaping? &lt;http://vita.had.co.nz/papers/tidy-data.html&gt;`_
+- Categoricals: WM 12.1</t>
   </si>
 </sst>
 </file>
@@ -817,7 +817,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,7 +1097,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="9"/>
     </row>
@@ -1109,7 +1109,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D22" s="8"/>
     </row>
@@ -1121,7 +1121,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="7"/>
     </row>

</xml_diff>

<commit_message>
update ex link for dask
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{401D9FDD-D2B1-C84E-9808-599CF2F74942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39265EB0-12CC-D046-82DD-3CD625E45E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
   <si>
     <t>Topic</t>
   </si>
@@ -427,6 +427,12 @@
   </si>
   <si>
     <t>- `Link &lt;execises/Exercise_codeyourownlinearregression.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;exercises/Exercise_dask_realdata.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>Catchup Time</t>
   </si>
 </sst>
 </file>
@@ -832,7 +838,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1212,11 +1218,16 @@
       <c r="C29" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="9"/>
+      <c r="D29" s="9" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>105</v>
       </c>
       <c r="D30" s="8"/>
     </row>

</xml_diff>